<commit_message>
Series Tipo de Cambio
</commit_message>
<xml_diff>
--- a/data/diccionario_cod.variable.xlsx
+++ b/data/diccionario_cod.variable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Guido\Trabajo\Repositorios de R\Repos Propios\ceped-data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA479314-33CB-4715-BD18-5360072708EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F703375-6359-4030-A9A7-2356C5199E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
   <si>
     <t>IPC_2005</t>
   </si>
@@ -98,6 +98,147 @@
   </si>
   <si>
     <t xml:space="preserve">Indice Salario real (2005 = 100) </t>
+  </si>
+  <si>
+    <t>TCNA_DL_Ferreres</t>
+  </si>
+  <si>
+    <t>TCNA_EXPO_Ferreres</t>
+  </si>
+  <si>
+    <t>TCNA_JIC</t>
+  </si>
+  <si>
+    <t>TCNA_Arceo</t>
+  </si>
+  <si>
+    <t>TCRA_2007_DL_Ferreres</t>
+  </si>
+  <si>
+    <t>TCRA_2007_EXPO_Ferreres</t>
+  </si>
+  <si>
+    <t>TCRA_2007_JIC</t>
+  </si>
+  <si>
+    <t>TCRA_2007_Arceo</t>
+  </si>
+  <si>
+    <t>Tipo de cambio nominal anual - Dólar Libre (Ferreres = Billetes Argentinos)</t>
+  </si>
+  <si>
+    <t>Tipo de cambio nominal anual - Dólar Exportaciones (Ferreres)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de cambio nominal anual - Iñigo Carrera </t>
+  </si>
+  <si>
+    <t>Tipo de cambio nominal anual - Arceo</t>
+  </si>
+  <si>
+    <t>Tipo_Cambio_Arg</t>
+  </si>
+  <si>
+    <t>Tipo de cambio real anual  (2007 = 100)- Dólar Libre (Ferreres = Billetes Argentinos)</t>
+  </si>
+  <si>
+    <t>Tipo de cambio real anual  (2007 = 100)- Dólar Exportaciones (Ferreres)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de cambio real anual  (2007 = 100)- Iñigo Carrera </t>
+  </si>
+  <si>
+    <t>Tipo de cambio real anual  (2007 = 100)- Arceo</t>
+  </si>
+  <si>
+    <t>Tipo de cambio de paridad anual - Metodología IPC - (Base-60-71) - Dólar Libre (Ferreres = Billetes Argentinos)</t>
+  </si>
+  <si>
+    <t>Tipo de cambio de paridad anual - Metodología IPC - (Base-60-71) - Dólar Exportaciones (Ferreres)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de cambio de paridad anual - Metodología IPC - (Base-60-71) - Iñigo Carrera </t>
+  </si>
+  <si>
+    <t>Tipo de cambio de paridad anual - Metodología IPC - (Base-60-71)  - Arceo</t>
+  </si>
+  <si>
+    <t>TCP_IPC_DL_Ferreres</t>
+  </si>
+  <si>
+    <t>TCP_IPC_EXPO_Ferreres</t>
+  </si>
+  <si>
+    <t>TCP_IPC_JIC</t>
+  </si>
+  <si>
+    <t>TCP_IPC_Arceo</t>
+  </si>
+  <si>
+    <t>TCP_IPC_PROD_DL_Ferreres</t>
+  </si>
+  <si>
+    <t>TCP_IPC_PROD_EXPO_Ferreres</t>
+  </si>
+  <si>
+    <t>TCP_IPC_PROD_JIC</t>
+  </si>
+  <si>
+    <t>TCP_IPC_PROD_Arceo</t>
+  </si>
+  <si>
+    <t>Tipo de cambio de paridad anual - Metodología IPC + Productividad - (Base-60-71) - Dólar Libre (Ferreres = Billetes Argentinos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de cambio de paridad anual - Metodología IPC + Productividad - (Base-60-71) - Iñigo Carrera </t>
+  </si>
+  <si>
+    <t>Tipo de cambio de paridad anual - Metodología IPC + Productividad - (Base-60-71)  - Arceo</t>
+  </si>
+  <si>
+    <t>GS_IPC_DL_Ferreres</t>
+  </si>
+  <si>
+    <t>GS_IPC_EXPO_Ferreres</t>
+  </si>
+  <si>
+    <t>GS_IPC_JIC</t>
+  </si>
+  <si>
+    <t>GS_IPC_Arceo</t>
+  </si>
+  <si>
+    <t>GS_IPC_PROD_DL_Ferreres</t>
+  </si>
+  <si>
+    <t>GS_IPC_PROD_EXPO_Ferreres</t>
+  </si>
+  <si>
+    <t>GS_IPC_PROD_JIC</t>
+  </si>
+  <si>
+    <t>GS_IPC_PROD_Arceo</t>
+  </si>
+  <si>
+    <t>Grado de sobrevaluación - Metodología IPC - (Base-60-71) - Dólar Libre (Ferreres = Billetes Argentinos)</t>
+  </si>
+  <si>
+    <t>Grado de sobrevaluación - Metodología IPC - (Base-60-71) - Dólar Exportaciones (Ferreres)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grado de sobrevaluación - Metodología IPC - (Base-60-71) - Iñigo Carrera </t>
+  </si>
+  <si>
+    <t>Grado de sobrevaluación - Metodología IPC - (Base-60-71)  - Arceo</t>
+  </si>
+  <si>
+    <t>Grado de sobrevaluación - Metodología IPC + Productividad - (Base-60-71) - Dólar Libre (Ferreres = Billetes Argentinos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grado de sobrevaluación - Metodología IPC + Productividad - (Base-60-71) - Iñigo Carrera </t>
+  </si>
+  <si>
+    <t>Grado de sobrevaluación - Metodología IPC + Productividad - (Base-60-71)  - Arceo</t>
   </si>
 </sst>
 </file>
@@ -431,7 +572,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -595,6 +736,270 @@
         <v>20</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>